<commit_message>
Update edited session - 2025-10-30T10:53:54.373Z - Cache Bust ID: 1761821634373id4c8cook
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2627_Biochemistry_Lab_CBL_scanner1761821577729_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
+++ b/log_history/Y3_B2627_Biochemistry_Lab_CBL_scanner1761821577729_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,29 +422,9 @@
         <v>User</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>222222</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Biochemistry Lab/CBL</v>
-      </c>
-      <c r="C2" t="str">
-        <v>30/10/2025</v>
-      </c>
-      <c r="D2" t="str">
-        <v>13:53:03</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F2" t="str">
-        <v>160715@med.asu.edu.eg</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>